<commit_message>
Installations and update of notes
</commit_message>
<xml_diff>
--- a/ExpenseTrackWinterNotes.xlsx
+++ b/ExpenseTrackWinterNotes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rgatc\Desktop\desktop\College\Spring-React\ExpenseTrackWinterGit\ExpenseTrackerTutorial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE7C04B2-8A78-42FB-90A3-A4C875C7F64F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C19E08A-0A90-47E1-90AF-2B6B0CD83B06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7200" yWindow="255" windowWidth="21600" windowHeight="11505" xr2:uid="{A6A4FEE8-7CE5-42A4-9EA4-5CD8B4E2CCC8}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
   <si>
     <t>spring.io</t>
   </si>
@@ -157,6 +157,24 @@
   </si>
   <si>
     <t>https://gitmemory.cn/index.php/repo/facebook/create-react-app/issues/11762</t>
+  </si>
+  <si>
+    <t>create Home.js</t>
+  </si>
+  <si>
+    <t>replace index.js to Home</t>
+  </si>
+  <si>
+    <t xml:space="preserve">npm install bootstrap </t>
+  </si>
+  <si>
+    <t>react-cookie</t>
+  </si>
+  <si>
+    <t>react-router-dom AND reactstrap</t>
+  </si>
+  <si>
+    <t>react-router routes between pages</t>
   </si>
 </sst>
 </file>
@@ -557,10 +575,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEB72CAD-DCEC-47F6-9651-15CEAD641395}">
-  <dimension ref="A1:F57"/>
+  <dimension ref="A1:F67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="M51" sqref="M51"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="M63" sqref="M63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -751,6 +769,32 @@
         <v>40</v>
       </c>
     </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>43</v>
+      </c>
+      <c r="D65" t="s">
+        <v>44</v>
+      </c>
+      <c r="F65" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>46</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>